<commit_message>
incremental updates to code and data
</commit_message>
<xml_diff>
--- a/outputs/version2/RIF_summary_2015-2020.xlsx
+++ b/outputs/version2/RIF_summary_2015-2020.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,23 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\mobility_fee_summary\outputs\version2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F38C8412-DBA3-495B-8249-DD814D0B580C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EC8337-1B67-45E1-BD97-6BA7F8174517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RIF_summary_2015-2020" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8715" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8710" uniqueCount="225">
   <si>
     <t>Ring</t>
   </si>
@@ -686,9 +697,6 @@
     <t>berth</t>
   </si>
   <si>
-    <t>(All)</t>
-  </si>
-  <si>
     <t>Grand Total</t>
   </si>
   <si>
@@ -707,7 +715,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1141,7 +1152,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1184,20 +1195,22 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1225,6 +1238,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="42" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1241,7 +1255,212 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="68">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1475,41 +1694,20 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>In</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>In</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
                     <c:v>Out</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>In</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Out</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>In</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
                     <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1517,27 +1715,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$15</c:f>
+              <c:f>Sheet1!$B$5:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-10703.598</c:v>
+                  <c:v>137474.91200000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-469490.06929999898</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-18568.308999999994</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-47953.906000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-101726.726</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>303784.44400000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1574,41 +1760,20 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>In</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>In</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
                     <c:v>Out</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>In</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Out</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>In</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
                     <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1616,27 +1781,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$15</c:f>
+              <c:f>Sheet1!$C$5:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>31510.219999999899</c:v>
+                  <c:v>1224913.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>82313.62</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>479529.67</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>81767.740000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1673,41 +1826,20 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>In</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>In</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
                     <c:v>Out</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>In</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Out</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>In</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
                     <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1715,27 +1847,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$15</c:f>
+              <c:f>Sheet1!$D$5:$D$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>55747.565999999999</c:v>
+                  <c:v>388798.56000000011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-371230.49599999993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1433291.6689599997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-579151.90119999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-51341.804360000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-59625.258000000002</c:v>
+                  <c:v>1057194.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1831,7 +1951,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2550,7 +2670,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Charles Rudder" refreshedDate="44398.617004861109" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="1449">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Charles Rudder" refreshedDate="44398.617004861109" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="1449" xr:uid="{00000000-000A-0000-FFFF-FFFF06000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:M1048576" sheet="RIF_summary_2015-2020"/>
   </cacheSource>
@@ -23907,15 +24027,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A4:D15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A4:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
       <items count="6">
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
         <item h="1" x="4"/>
         <item t="default"/>
       </items>
@@ -23934,9 +24054,9 @@
       <items count="80">
         <item h="1" x="9"/>
         <item h="1" x="48"/>
-        <item h="1" x="4"/>
+        <item x="4"/>
         <item h="1" x="51"/>
-        <item x="46"/>
+        <item h="1" x="46"/>
         <item h="1" x="30"/>
         <item h="1" x="43"/>
         <item h="1" x="29"/>
@@ -24940,15 +25060,15 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisPage" showAll="0">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="8">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
         <item x="5"/>
-        <item x="6"/>
+        <item h="1" x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -24957,13 +25077,7 @@
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
+  <rowItems count="4">
     <i>
       <x v="1"/>
     </i>
@@ -24972,21 +25086,6 @@
     </i>
     <i r="1">
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x/>
     </i>
     <i t="grand">
       <x/>
@@ -25015,6 +25114,241 @@
     <dataField name="Sum of ROAD_IMPACT_FEE" fld="8" baseField="0" baseItem="0"/>
     <dataField name="Sum of MF_RT_BASED_FEE" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="17">
+    <format dxfId="67">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="66">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="59">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="57">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="56">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="55">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="54">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="53">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="52">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="51">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
@@ -25352,7 +25686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1449"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -84771,10 +85105,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -85388,8 +85724,8 @@
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>220</v>
+      <c r="B1" s="3">
+        <v>2020</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -85397,175 +85733,83 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" t="s">
         <v>222</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>223</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>224</v>
-      </c>
-      <c r="D4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4">
-        <v>-10703.598</v>
-      </c>
-      <c r="C5" s="4">
-        <v>31510.219999999899</v>
-      </c>
-      <c r="D5" s="4">
-        <v>55747.565999999999</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>441259.35600000003</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1306681.23</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1445992.8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4">
-        <v>-10703.598</v>
-      </c>
-      <c r="C6" s="4">
-        <v>31510.219999999899</v>
-      </c>
-      <c r="D6" s="4">
-        <v>55747.565999999999</v>
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5">
+        <v>137474.91200000001</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1224913.49</v>
+      </c>
+      <c r="D6" s="5">
+        <v>388798.56000000011</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4">
-        <v>-488058.37829999899</v>
-      </c>
-      <c r="C7" s="4">
-        <v>82313.62</v>
-      </c>
-      <c r="D7" s="4">
-        <v>-1804522.1649599997</v>
+      <c r="A7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="5">
+        <v>303784.44400000002</v>
+      </c>
+      <c r="C7" s="5">
+        <v>81767.740000000005</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1057194.24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4">
-        <v>-469490.06929999898</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>-371230.49599999993</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="4">
-        <v>-18568.308999999994</v>
-      </c>
-      <c r="C9" s="4">
-        <v>82313.62</v>
-      </c>
-      <c r="D9" s="4">
-        <v>-1433291.6689599997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4">
-        <v>-149680.63199999998</v>
-      </c>
-      <c r="C10" s="4">
-        <v>479529.67</v>
-      </c>
-      <c r="D10" s="4">
-        <v>-630493.70555999991</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4">
-        <v>-47953.906000000003</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>-579151.90119999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="4">
-        <v>-101726.726</v>
-      </c>
-      <c r="C12" s="4">
-        <v>479529.67</v>
-      </c>
-      <c r="D12" s="4">
-        <v>-51341.804360000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>4</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>-59625.258000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>-59625.258000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B15" s="4">
-        <v>-648442.60829999903</v>
-      </c>
-      <c r="C15" s="4">
-        <v>593353.50999999989</v>
-      </c>
-      <c r="D15" s="4">
-        <v>-2438893.5625199992</v>
+      <c r="A8" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" s="5">
+        <v>441259.35600000003</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1306681.23</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1445992.8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="6">
+        <f>GETPIVOTDATA("Sum of ROAD_IMPACT_FEE",$A$4)-GETPIVOTDATA("Sum of MF_RT_BASED_FEE",$A$4)</f>
+        <v>-139311.57000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>